<commit_message>
updated patient log for newest case of tamponade
</commit_message>
<xml_diff>
--- a/docs/log.xlsx
+++ b/docs/log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emory-my.sharepoint.com/personal/asshah4_emory_edu/Documents/projects/patient-log/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="423" documentId="13_ncr:1_{3CB9D789-FF1C-4735-9260-A83070EE7DFA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B5596E72-A090-45AB-B9E9-08F30C4342F3}"/>
+  <xr:revisionPtr revIDLastSave="536" documentId="13_ncr:1_{3CB9D789-FF1C-4735-9260-A83070EE7DFA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{9A216A20-7106-4A2A-8093-C9C96029C346}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3191" uniqueCount="563">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3314" uniqueCount="590">
   <si>
     <t>SITE</t>
   </si>
@@ -1719,6 +1719,87 @@
   </si>
   <si>
     <t>031174840</t>
+  </si>
+  <si>
+    <t>081514530</t>
+  </si>
+  <si>
+    <t>081550797</t>
+  </si>
+  <si>
+    <t>VSD</t>
+  </si>
+  <si>
+    <t>076462787</t>
+  </si>
+  <si>
+    <t>087054912</t>
+  </si>
+  <si>
+    <t>071434237</t>
+  </si>
+  <si>
+    <t>071991053</t>
+  </si>
+  <si>
+    <t>080911553</t>
+  </si>
+  <si>
+    <t>2000103647</t>
+  </si>
+  <si>
+    <t>080684682</t>
+  </si>
+  <si>
+    <t>200206802</t>
+  </si>
+  <si>
+    <t>051365492</t>
+  </si>
+  <si>
+    <t>081068545</t>
+  </si>
+  <si>
+    <t>007737547</t>
+  </si>
+  <si>
+    <t>081553125</t>
+  </si>
+  <si>
+    <t>080715006</t>
+  </si>
+  <si>
+    <t>080708793</t>
+  </si>
+  <si>
+    <t>081528442</t>
+  </si>
+  <si>
+    <t>070931852</t>
+  </si>
+  <si>
+    <t>080905668</t>
+  </si>
+  <si>
+    <t>080073902</t>
+  </si>
+  <si>
+    <t>051582518</t>
+  </si>
+  <si>
+    <t>077069367</t>
+  </si>
+  <si>
+    <t>081276913</t>
+  </si>
+  <si>
+    <t>076821909</t>
+  </si>
+  <si>
+    <t>081546846</t>
+  </si>
+  <si>
+    <t>W6561</t>
   </si>
 </sst>
 </file>
@@ -2093,11 +2174,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I647"/>
+  <dimension ref="A1:I678"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="165" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A638" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B648" sqref="B648"/>
+      <pane ySplit="1" topLeftCell="A675" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E679" sqref="E679"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -15947,6 +16028,9 @@
       </c>
     </row>
     <row r="647" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A647" t="s">
+        <v>9</v>
+      </c>
       <c r="B647" s="4" t="s">
         <v>562</v>
       </c>
@@ -15955,6 +16039,527 @@
       </c>
       <c r="G647" t="s">
         <v>80</v>
+      </c>
+    </row>
+    <row r="648" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A648" t="s">
+        <v>9</v>
+      </c>
+      <c r="B648" s="4" t="s">
+        <v>563</v>
+      </c>
+      <c r="C648" s="1">
+        <v>44181</v>
+      </c>
+      <c r="D648" t="s">
+        <v>193</v>
+      </c>
+      <c r="E648" t="s">
+        <v>60</v>
+      </c>
+      <c r="G648" t="s">
+        <v>75</v>
+      </c>
+      <c r="H648" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="649" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A649" t="s">
+        <v>9</v>
+      </c>
+      <c r="B649" s="4" t="s">
+        <v>563</v>
+      </c>
+      <c r="C649" s="1">
+        <v>44181</v>
+      </c>
+      <c r="D649" t="s">
+        <v>193</v>
+      </c>
+      <c r="E649" t="s">
+        <v>60</v>
+      </c>
+      <c r="G649" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="650" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A650" t="s">
+        <v>9</v>
+      </c>
+      <c r="B650" s="4" t="s">
+        <v>564</v>
+      </c>
+      <c r="C650" s="1">
+        <v>44181</v>
+      </c>
+      <c r="D650" t="s">
+        <v>565</v>
+      </c>
+      <c r="E650" t="s">
+        <v>445</v>
+      </c>
+      <c r="G650" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="651" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A651" t="s">
+        <v>9</v>
+      </c>
+      <c r="B651" s="4" t="s">
+        <v>566</v>
+      </c>
+      <c r="C651" s="1">
+        <v>44180</v>
+      </c>
+      <c r="G651" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="652" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A652" t="s">
+        <v>9</v>
+      </c>
+      <c r="B652" s="4" t="s">
+        <v>567</v>
+      </c>
+      <c r="C652" s="1">
+        <v>44180</v>
+      </c>
+      <c r="G652" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="653" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A653" t="s">
+        <v>9</v>
+      </c>
+      <c r="B653" s="4" t="s">
+        <v>568</v>
+      </c>
+      <c r="C653" s="1">
+        <v>44180</v>
+      </c>
+      <c r="G653" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="654" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A654" t="s">
+        <v>9</v>
+      </c>
+      <c r="B654" s="4" t="s">
+        <v>569</v>
+      </c>
+      <c r="C654" s="1">
+        <v>44180</v>
+      </c>
+      <c r="G654" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="655" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A655" t="s">
+        <v>9</v>
+      </c>
+      <c r="B655" s="4" t="s">
+        <v>570</v>
+      </c>
+      <c r="C655" s="1">
+        <v>44180</v>
+      </c>
+      <c r="D655" t="s">
+        <v>260</v>
+      </c>
+      <c r="G655" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="656" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A656" t="s">
+        <v>9</v>
+      </c>
+      <c r="B656" s="4" t="s">
+        <v>564</v>
+      </c>
+      <c r="C656" s="1">
+        <v>44181</v>
+      </c>
+      <c r="G656" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="657" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A657" t="s">
+        <v>9</v>
+      </c>
+      <c r="B657" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="C657" s="1">
+        <v>44181</v>
+      </c>
+      <c r="G657" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="658" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A658" t="s">
+        <v>9</v>
+      </c>
+      <c r="B658" s="4" t="s">
+        <v>572</v>
+      </c>
+      <c r="C658" s="1">
+        <v>44181</v>
+      </c>
+      <c r="G658" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="659" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A659" t="s">
+        <v>9</v>
+      </c>
+      <c r="B659" s="4" t="s">
+        <v>573</v>
+      </c>
+      <c r="C659" s="1">
+        <v>44181</v>
+      </c>
+      <c r="G659" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="660" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A660" t="s">
+        <v>9</v>
+      </c>
+      <c r="B660" s="4" t="s">
+        <v>574</v>
+      </c>
+      <c r="C660" s="1">
+        <v>44181</v>
+      </c>
+      <c r="G660" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="661" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A661" t="s">
+        <v>9</v>
+      </c>
+      <c r="B661" s="4" t="s">
+        <v>575</v>
+      </c>
+      <c r="C661" s="1">
+        <v>44181</v>
+      </c>
+      <c r="G661" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="662" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A662" t="s">
+        <v>9</v>
+      </c>
+      <c r="B662" s="4" t="s">
+        <v>576</v>
+      </c>
+      <c r="C662" s="1">
+        <v>44181</v>
+      </c>
+      <c r="G662" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="663" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A663" t="s">
+        <v>9</v>
+      </c>
+      <c r="B663" s="4" t="s">
+        <v>577</v>
+      </c>
+      <c r="C663" s="1">
+        <v>44181</v>
+      </c>
+      <c r="G663" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="664" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A664" t="s">
+        <v>9</v>
+      </c>
+      <c r="B664" s="4" t="s">
+        <v>578</v>
+      </c>
+      <c r="C664" s="1">
+        <v>44181</v>
+      </c>
+      <c r="G664" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="665" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A665" t="s">
+        <v>9</v>
+      </c>
+      <c r="B665" s="4" t="s">
+        <v>579</v>
+      </c>
+      <c r="C665" s="1">
+        <v>44181</v>
+      </c>
+      <c r="G665" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="666" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A666" t="s">
+        <v>9</v>
+      </c>
+      <c r="B666" s="4" t="s">
+        <v>580</v>
+      </c>
+      <c r="C666" s="1">
+        <v>44181</v>
+      </c>
+      <c r="G666" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="667" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A667" t="s">
+        <v>9</v>
+      </c>
+      <c r="B667" s="4" t="s">
+        <v>581</v>
+      </c>
+      <c r="C667" s="1">
+        <v>44181</v>
+      </c>
+      <c r="G667" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="668" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A668" t="s">
+        <v>9</v>
+      </c>
+      <c r="B668" s="4" t="s">
+        <v>582</v>
+      </c>
+      <c r="C668" s="1">
+        <v>44181</v>
+      </c>
+      <c r="G668" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="669" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A669" t="s">
+        <v>9</v>
+      </c>
+      <c r="B669" s="4" t="s">
+        <v>583</v>
+      </c>
+      <c r="C669" s="1">
+        <v>44181</v>
+      </c>
+      <c r="D669" t="s">
+        <v>49</v>
+      </c>
+      <c r="E669" t="s">
+        <v>10</v>
+      </c>
+      <c r="G669" t="s">
+        <v>75</v>
+      </c>
+      <c r="H669" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="670" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A670" t="s">
+        <v>9</v>
+      </c>
+      <c r="B670" s="4" t="s">
+        <v>583</v>
+      </c>
+      <c r="C670" s="1">
+        <v>44181</v>
+      </c>
+      <c r="D670" t="s">
+        <v>49</v>
+      </c>
+      <c r="E670" t="s">
+        <v>10</v>
+      </c>
+      <c r="G670" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="671" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A671" t="s">
+        <v>9</v>
+      </c>
+      <c r="B671" s="4" t="s">
+        <v>583</v>
+      </c>
+      <c r="C671" s="1">
+        <v>44181</v>
+      </c>
+      <c r="D671" t="s">
+        <v>49</v>
+      </c>
+      <c r="E671" t="s">
+        <v>10</v>
+      </c>
+      <c r="G671" t="s">
+        <v>86</v>
+      </c>
+      <c r="H671" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="672" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A672" t="s">
+        <v>9</v>
+      </c>
+      <c r="B672" s="4" t="s">
+        <v>584</v>
+      </c>
+      <c r="C672" s="1">
+        <v>44181</v>
+      </c>
+      <c r="G672" t="s">
+        <v>80</v>
+      </c>
+      <c r="I672" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="673" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A673" t="s">
+        <v>9</v>
+      </c>
+      <c r="B673" s="4" t="s">
+        <v>585</v>
+      </c>
+      <c r="C673" s="1">
+        <v>44181</v>
+      </c>
+      <c r="D673" t="s">
+        <v>271</v>
+      </c>
+      <c r="G673" t="s">
+        <v>125</v>
+      </c>
+      <c r="H673" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="674" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A674" t="s">
+        <v>9</v>
+      </c>
+      <c r="B674" s="4" t="s">
+        <v>586</v>
+      </c>
+      <c r="C674" s="1">
+        <v>44181</v>
+      </c>
+      <c r="D674" t="s">
+        <v>271</v>
+      </c>
+      <c r="G674" t="s">
+        <v>125</v>
+      </c>
+      <c r="H674" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="675" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A675" t="s">
+        <v>9</v>
+      </c>
+      <c r="B675" s="4" t="s">
+        <v>579</v>
+      </c>
+      <c r="C675" s="1">
+        <v>44181</v>
+      </c>
+      <c r="D675" t="s">
+        <v>271</v>
+      </c>
+      <c r="G675" t="s">
+        <v>125</v>
+      </c>
+      <c r="H675" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="676" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A676" t="s">
+        <v>9</v>
+      </c>
+      <c r="B676" s="4" t="s">
+        <v>587</v>
+      </c>
+      <c r="C676" s="1">
+        <v>44181</v>
+      </c>
+      <c r="D676" t="s">
+        <v>249</v>
+      </c>
+      <c r="G676" t="s">
+        <v>125</v>
+      </c>
+      <c r="H676" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="677" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A677" t="s">
+        <v>9</v>
+      </c>
+      <c r="B677" s="4" t="s">
+        <v>588</v>
+      </c>
+      <c r="C677" s="1">
+        <v>44181</v>
+      </c>
+      <c r="D677" t="s">
+        <v>271</v>
+      </c>
+      <c r="G677" t="s">
+        <v>125</v>
+      </c>
+      <c r="H677" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="678" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A678" t="s">
+        <v>65</v>
+      </c>
+      <c r="B678" s="4" t="s">
+        <v>589</v>
+      </c>
+      <c r="C678" s="1">
+        <v>44183</v>
+      </c>
+      <c r="D678" t="s">
+        <v>24</v>
+      </c>
+      <c r="E678" t="s">
+        <v>142</v>
+      </c>
+      <c r="H678" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated paths, built tentative site, sending for prelim review of JC
</commit_message>
<xml_diff>
--- a/docs/log.xlsx
+++ b/docs/log.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emory-my.sharepoint.com/personal/asshah4_emory_edu/Documents/projects/patient-log/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emory-my.sharepoint.com/personal/asshah4_emory_edu/Documents/projects/clinical/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="536" documentId="13_ncr:1_{3CB9D789-FF1C-4735-9260-A83070EE7DFA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{9A216A20-7106-4A2A-8093-C9C96029C346}"/>
+  <xr:revisionPtr revIDLastSave="1123" documentId="13_ncr:1_{3CB9D789-FF1C-4735-9260-A83070EE7DFA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{1E78F8FE-72CE-49BB-8F70-8B592D4AEF15}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3314" uniqueCount="590">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3901" uniqueCount="720">
   <si>
     <t>SITE</t>
   </si>
@@ -1800,13 +1800,403 @@
   </si>
   <si>
     <t>W6561</t>
+  </si>
+  <si>
+    <t>ACMC</t>
+  </si>
+  <si>
+    <t>5092331</t>
+  </si>
+  <si>
+    <t>VAD</t>
+  </si>
+  <si>
+    <t>respiratory failure</t>
+  </si>
+  <si>
+    <t>11483621</t>
+  </si>
+  <si>
+    <t>10327055</t>
+  </si>
+  <si>
+    <t>heart transplant</t>
+  </si>
+  <si>
+    <t>procurement</t>
+  </si>
+  <si>
+    <t>11472843</t>
+  </si>
+  <si>
+    <t>ECMO</t>
+  </si>
+  <si>
+    <t>11494242</t>
+  </si>
+  <si>
+    <t>11000204</t>
+  </si>
+  <si>
+    <t>11469706</t>
+  </si>
+  <si>
+    <t>11113585</t>
+  </si>
+  <si>
+    <t>11467575</t>
+  </si>
+  <si>
+    <t>tracheomalacia</t>
+  </si>
+  <si>
+    <t>5457023</t>
+  </si>
+  <si>
+    <t>central stenosis</t>
+  </si>
+  <si>
+    <t>7207975</t>
+  </si>
+  <si>
+    <t>7059295</t>
+  </si>
+  <si>
+    <t>DC-ICD</t>
+  </si>
+  <si>
+    <t>9552531</t>
+  </si>
+  <si>
+    <t>J1260</t>
+  </si>
+  <si>
+    <t>S0769</t>
+  </si>
+  <si>
+    <t>W1358</t>
+  </si>
+  <si>
+    <t>I5512</t>
+  </si>
+  <si>
+    <t>N0677</t>
+  </si>
+  <si>
+    <t>nonagenarian</t>
+  </si>
+  <si>
+    <t>A121120</t>
+  </si>
+  <si>
+    <t>M121120</t>
+  </si>
+  <si>
+    <t>troponinemia</t>
+  </si>
+  <si>
+    <t>H121120</t>
+  </si>
+  <si>
+    <t>PDS</t>
+  </si>
+  <si>
+    <t>L121120</t>
+  </si>
+  <si>
+    <t>S121120</t>
+  </si>
+  <si>
+    <t>MM</t>
+  </si>
+  <si>
+    <t>W121020</t>
+  </si>
+  <si>
+    <t>LQTS</t>
+  </si>
+  <si>
+    <t>O120920</t>
+  </si>
+  <si>
+    <t>M121020</t>
+  </si>
+  <si>
+    <t>LVH</t>
+  </si>
+  <si>
+    <t>004056883</t>
+  </si>
+  <si>
+    <t>D121020</t>
+  </si>
+  <si>
+    <t>L9125</t>
+  </si>
+  <si>
+    <t>ERS</t>
+  </si>
+  <si>
+    <t>SPECIAL</t>
+  </si>
+  <si>
+    <t>K11469706</t>
+  </si>
+  <si>
+    <t>pneumonia</t>
+  </si>
+  <si>
+    <t>7034118</t>
+  </si>
+  <si>
+    <t>goiter</t>
+  </si>
+  <si>
+    <t>071386635</t>
+  </si>
+  <si>
+    <t>T01192021</t>
+  </si>
+  <si>
+    <t>pancreatic cancer</t>
+  </si>
+  <si>
+    <t>200250881</t>
+  </si>
+  <si>
+    <t>200250457</t>
+  </si>
+  <si>
+    <t>070748082</t>
+  </si>
+  <si>
+    <t>080343926</t>
+  </si>
+  <si>
+    <t>200252952</t>
+  </si>
+  <si>
+    <t>081084674</t>
+  </si>
+  <si>
+    <t>007706112</t>
+  </si>
+  <si>
+    <t>081045218</t>
+  </si>
+  <si>
+    <t>200252941</t>
+  </si>
+  <si>
+    <t>075021113</t>
+  </si>
+  <si>
+    <t>081126674</t>
+  </si>
+  <si>
+    <t>072024482</t>
+  </si>
+  <si>
+    <t>010090173</t>
+  </si>
+  <si>
+    <t>010519528</t>
+  </si>
+  <si>
+    <t>200198511</t>
+  </si>
+  <si>
+    <t>072857782</t>
+  </si>
+  <si>
+    <t>07003582</t>
+  </si>
+  <si>
+    <t>200105414</t>
+  </si>
+  <si>
+    <t>081181237</t>
+  </si>
+  <si>
+    <t>081216287</t>
+  </si>
+  <si>
+    <t>081088961</t>
+  </si>
+  <si>
+    <t>073073553</t>
+  </si>
+  <si>
+    <t>081144088</t>
+  </si>
+  <si>
+    <t>VF arrest</t>
+  </si>
+  <si>
+    <t>CO2 embolus</t>
+  </si>
+  <si>
+    <t>081562242</t>
+  </si>
+  <si>
+    <t>081510265</t>
+  </si>
+  <si>
+    <t>081274803</t>
+  </si>
+  <si>
+    <t>087024006</t>
+  </si>
+  <si>
+    <t>070786439</t>
+  </si>
+  <si>
+    <t>080944677</t>
+  </si>
+  <si>
+    <t>080929572</t>
+  </si>
+  <si>
+    <t>070413000</t>
+  </si>
+  <si>
+    <t>200254068</t>
+  </si>
+  <si>
+    <t>070374657</t>
+  </si>
+  <si>
+    <t>200213756</t>
+  </si>
+  <si>
+    <t>200210186</t>
+  </si>
+  <si>
+    <t>070797063</t>
+  </si>
+  <si>
+    <t>081057619</t>
+  </si>
+  <si>
+    <t>lupus</t>
+  </si>
+  <si>
+    <t>200252739</t>
+  </si>
+  <si>
+    <t>080678498</t>
+  </si>
+  <si>
+    <t>071195267</t>
+  </si>
+  <si>
+    <t>200199768</t>
+  </si>
+  <si>
+    <t>075697052</t>
+  </si>
+  <si>
+    <t>080337430</t>
+  </si>
+  <si>
+    <t>087088449</t>
+  </si>
+  <si>
+    <t>200254423</t>
+  </si>
+  <si>
+    <t>080936335</t>
+  </si>
+  <si>
+    <t>080117366</t>
+  </si>
+  <si>
+    <t>080021471</t>
+  </si>
+  <si>
+    <t>081155573</t>
+  </si>
+  <si>
+    <t>081450956</t>
+  </si>
+  <si>
+    <t>081482602</t>
+  </si>
+  <si>
+    <t>200253384</t>
+  </si>
+  <si>
+    <t>081520194</t>
+  </si>
+  <si>
+    <t>080655007</t>
+  </si>
+  <si>
+    <t>081482161</t>
+  </si>
+  <si>
+    <t>051641983</t>
+  </si>
+  <si>
+    <t>200256419</t>
+  </si>
+  <si>
+    <t>081323814</t>
+  </si>
+  <si>
+    <t>structural</t>
+  </si>
+  <si>
+    <t>200195082</t>
+  </si>
+  <si>
+    <t>081548675</t>
+  </si>
+  <si>
+    <t>080310420</t>
+  </si>
+  <si>
+    <t>200106873</t>
+  </si>
+  <si>
+    <t>080878880</t>
+  </si>
+  <si>
+    <t>072952948</t>
+  </si>
+  <si>
+    <t>200255391</t>
+  </si>
+  <si>
+    <t>006640692</t>
+  </si>
+  <si>
+    <t>073052763</t>
+  </si>
+  <si>
+    <t>050988922</t>
+  </si>
+  <si>
+    <t>074413352</t>
+  </si>
+  <si>
+    <t>081551473</t>
+  </si>
+  <si>
+    <t>080606193</t>
+  </si>
+  <si>
+    <t>200255583</t>
+  </si>
+  <si>
+    <t>031295212</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1817,6 +2207,13 @@
     <font>
       <sz val="11"/>
       <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1851,7 +2248,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1860,6 +2257,9 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2174,11 +2574,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I678"/>
+  <dimension ref="A1:J810"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="165" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A675" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E679" sqref="E679"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A794" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D807" sqref="D807"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2187,9 +2587,10 @@
     <col min="2" max="2" width="12.1796875" style="4" customWidth="1"/>
     <col min="3" max="3" width="10.6328125" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="17" customWidth="1"/>
+    <col min="9" max="9" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2217,8 +2618,11 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J1" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -2247,7 +2651,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -2276,7 +2680,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -2299,7 +2703,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -2325,7 +2729,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -2351,7 +2755,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -2380,7 +2784,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -2406,7 +2810,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -2432,7 +2836,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -2458,7 +2862,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -2484,7 +2888,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -2510,7 +2914,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -2539,7 +2943,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -2568,7 +2972,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -2597,7 +3001,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -8100,7 +8504,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="273" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A273" t="s">
         <v>9</v>
       </c>
@@ -8126,7 +8530,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="274" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A274" t="s">
         <v>9</v>
       </c>
@@ -8152,7 +8556,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="275" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A275" t="s">
         <v>9</v>
       </c>
@@ -8178,7 +8582,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="276" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A276" t="s">
         <v>9</v>
       </c>
@@ -8204,7 +8608,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="277" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A277" t="s">
         <v>9</v>
       </c>
@@ -8230,7 +8634,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="278" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A278" t="s">
         <v>9</v>
       </c>
@@ -8256,7 +8660,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="279" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A279" t="s">
         <v>9</v>
       </c>
@@ -8282,7 +8686,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="280" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A280" t="s">
         <v>9</v>
       </c>
@@ -8311,7 +8715,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="281" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A281" t="s">
         <v>9</v>
       </c>
@@ -8340,7 +8744,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="282" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A282" t="s">
         <v>9</v>
       </c>
@@ -8369,7 +8773,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="283" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A283" t="s">
         <v>9</v>
       </c>
@@ -8395,7 +8799,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="284" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A284" s="2" t="s">
         <v>9</v>
       </c>
@@ -8421,7 +8825,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="285" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A285" s="3" t="s">
         <v>9</v>
       </c>
@@ -8446,8 +8850,11 @@
       <c r="I285" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="286" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J285">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="286" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A286" s="3" t="s">
         <v>9</v>
       </c>
@@ -8467,7 +8874,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="287" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A287" s="3" t="s">
         <v>9</v>
       </c>
@@ -8490,7 +8897,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="288" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A288" s="3" t="s">
         <v>9</v>
       </c>
@@ -10873,7 +11280,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="401" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="401" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A401" s="3" t="s">
         <v>65</v>
       </c>
@@ -10890,7 +11297,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="402" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="402" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A402" s="3" t="s">
         <v>65</v>
       </c>
@@ -10910,7 +11317,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="403" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="403" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A403" s="3" t="s">
         <v>65</v>
       </c>
@@ -10930,7 +11337,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="404" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="404" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A404" s="3" t="s">
         <v>65</v>
       </c>
@@ -10944,7 +11351,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="405" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="405" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A405" s="3" t="s">
         <v>9</v>
       </c>
@@ -10967,7 +11374,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="406" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="406" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A406" s="3" t="s">
         <v>9</v>
       </c>
@@ -10996,7 +11403,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="407" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="407" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A407" s="3" t="s">
         <v>9</v>
       </c>
@@ -11025,7 +11432,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="408" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="408" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A408" s="3" t="s">
         <v>9</v>
       </c>
@@ -11048,7 +11455,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="409" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="409" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A409" s="3" t="s">
         <v>9</v>
       </c>
@@ -11073,8 +11480,11 @@
       <c r="I409" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="410" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J409">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="410" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A410" s="3" t="s">
         <v>9</v>
       </c>
@@ -11100,7 +11510,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="411" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="411" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A411" s="3" t="s">
         <v>9</v>
       </c>
@@ -11129,7 +11539,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="412" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="412" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A412" s="3" t="s">
         <v>65</v>
       </c>
@@ -11152,7 +11562,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="413" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="413" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A413" s="3" t="s">
         <v>65</v>
       </c>
@@ -11172,7 +11582,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="414" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="414" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A414" s="3" t="s">
         <v>65</v>
       </c>
@@ -11186,7 +11596,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="415" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="415" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A415" s="3" t="s">
         <v>65</v>
       </c>
@@ -11200,7 +11610,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="416" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="416" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A416" s="3" t="s">
         <v>65</v>
       </c>
@@ -15518,7 +15928,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="625" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="625" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A625" t="s">
         <v>65</v>
       </c>
@@ -15541,7 +15951,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="626" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="626" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A626" t="s">
         <v>65</v>
       </c>
@@ -15564,7 +15974,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="627" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="627" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A627" t="s">
         <v>65</v>
       </c>
@@ -15586,8 +15996,11 @@
       <c r="I627" t="s">
         <v>542</v>
       </c>
-    </row>
-    <row r="628" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J627">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="628" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A628" t="s">
         <v>65</v>
       </c>
@@ -15610,7 +16023,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="629" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="629" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A629" t="s">
         <v>65</v>
       </c>
@@ -15633,7 +16046,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="630" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="630" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A630" t="s">
         <v>543</v>
       </c>
@@ -15656,7 +16069,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="631" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="631" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A631" t="s">
         <v>65</v>
       </c>
@@ -15682,7 +16095,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="632" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="632" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A632" t="s">
         <v>65</v>
       </c>
@@ -15705,7 +16118,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="633" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="633" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A633" t="s">
         <v>65</v>
       </c>
@@ -15725,7 +16138,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="634" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="634" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A634" t="s">
         <v>65</v>
       </c>
@@ -15751,7 +16164,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="635" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="635" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A635" t="s">
         <v>65</v>
       </c>
@@ -15774,7 +16187,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="636" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="636" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A636" t="s">
         <v>9</v>
       </c>
@@ -15788,7 +16201,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="637" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="637" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A637" t="s">
         <v>9</v>
       </c>
@@ -15817,7 +16230,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="638" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="638" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A638" t="s">
         <v>9</v>
       </c>
@@ -15840,7 +16253,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="639" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="639" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A639" t="s">
         <v>9</v>
       </c>
@@ -15866,7 +16279,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="640" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="640" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A640" t="s">
         <v>9</v>
       </c>
@@ -16442,7 +16855,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="673" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="673" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A673" t="s">
         <v>9</v>
       </c>
@@ -16462,7 +16875,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="674" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="674" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A674" t="s">
         <v>9</v>
       </c>
@@ -16482,7 +16895,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="675" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="675" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A675" t="s">
         <v>9</v>
       </c>
@@ -16502,7 +16915,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="676" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="676" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A676" t="s">
         <v>9</v>
       </c>
@@ -16522,7 +16935,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="677" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="677" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A677" t="s">
         <v>9</v>
       </c>
@@ -16542,7 +16955,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="678" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="678" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A678" t="s">
         <v>65</v>
       </c>
@@ -16560,6 +16973,2439 @@
       </c>
       <c r="H678" t="s">
         <v>69</v>
+      </c>
+    </row>
+    <row r="679" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A679" t="s">
+        <v>590</v>
+      </c>
+      <c r="B679" s="4" t="s">
+        <v>591</v>
+      </c>
+      <c r="C679" s="1">
+        <v>44204</v>
+      </c>
+      <c r="D679" t="s">
+        <v>592</v>
+      </c>
+      <c r="E679" t="s">
+        <v>167</v>
+      </c>
+      <c r="F679" t="s">
+        <v>593</v>
+      </c>
+      <c r="G679" t="s">
+        <v>269</v>
+      </c>
+      <c r="H679" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="680" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A680" t="s">
+        <v>590</v>
+      </c>
+      <c r="B680" s="4" t="s">
+        <v>591</v>
+      </c>
+      <c r="C680" s="1">
+        <v>44204</v>
+      </c>
+      <c r="D680" t="s">
+        <v>592</v>
+      </c>
+      <c r="E680" t="s">
+        <v>167</v>
+      </c>
+      <c r="F680" t="s">
+        <v>593</v>
+      </c>
+      <c r="G680" t="s">
+        <v>477</v>
+      </c>
+      <c r="H680" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="681" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A681" t="s">
+        <v>590</v>
+      </c>
+      <c r="B681" s="4" t="s">
+        <v>594</v>
+      </c>
+      <c r="C681" s="1">
+        <v>44203</v>
+      </c>
+      <c r="D681" t="s">
+        <v>358</v>
+      </c>
+      <c r="E681" t="s">
+        <v>51</v>
+      </c>
+      <c r="G681" t="s">
+        <v>269</v>
+      </c>
+      <c r="H681" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="682" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A682" t="s">
+        <v>590</v>
+      </c>
+      <c r="B682" s="4" t="s">
+        <v>594</v>
+      </c>
+      <c r="C682" s="1">
+        <v>44203</v>
+      </c>
+      <c r="D682" t="s">
+        <v>358</v>
+      </c>
+      <c r="E682" t="s">
+        <v>51</v>
+      </c>
+      <c r="G682" t="s">
+        <v>477</v>
+      </c>
+      <c r="H682" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="683" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A683" t="s">
+        <v>590</v>
+      </c>
+      <c r="B683" s="8" t="s">
+        <v>594</v>
+      </c>
+      <c r="C683" s="9">
+        <v>44203</v>
+      </c>
+      <c r="D683" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="E683" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F683" s="10"/>
+      <c r="G683" s="10"/>
+      <c r="H683" t="s">
+        <v>150</v>
+      </c>
+      <c r="J683">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="684" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A684" t="s">
+        <v>590</v>
+      </c>
+      <c r="B684" s="4" t="s">
+        <v>595</v>
+      </c>
+      <c r="C684" s="1">
+        <v>44201</v>
+      </c>
+      <c r="D684" t="s">
+        <v>51</v>
+      </c>
+      <c r="E684" t="s">
+        <v>592</v>
+      </c>
+      <c r="F684" t="s">
+        <v>596</v>
+      </c>
+      <c r="H684" t="s">
+        <v>150</v>
+      </c>
+      <c r="I684" t="s">
+        <v>597</v>
+      </c>
+      <c r="J684">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="685" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A685" t="s">
+        <v>590</v>
+      </c>
+      <c r="B685" s="4" t="s">
+        <v>598</v>
+      </c>
+      <c r="C685" s="1">
+        <v>44202</v>
+      </c>
+      <c r="D685" t="s">
+        <v>24</v>
+      </c>
+      <c r="E685" t="s">
+        <v>51</v>
+      </c>
+      <c r="F685" t="s">
+        <v>599</v>
+      </c>
+      <c r="H685" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="686" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A686" t="s">
+        <v>590</v>
+      </c>
+      <c r="B686" s="4" t="s">
+        <v>600</v>
+      </c>
+      <c r="C686" s="1">
+        <v>44203</v>
+      </c>
+      <c r="D686" t="s">
+        <v>51</v>
+      </c>
+      <c r="E686" t="s">
+        <v>263</v>
+      </c>
+      <c r="F686" t="s">
+        <v>599</v>
+      </c>
+      <c r="H686" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="687" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A687" t="s">
+        <v>590</v>
+      </c>
+      <c r="B687" s="4" t="s">
+        <v>601</v>
+      </c>
+      <c r="C687" s="1">
+        <v>44202</v>
+      </c>
+      <c r="D687" t="s">
+        <v>51</v>
+      </c>
+      <c r="E687" t="s">
+        <v>60</v>
+      </c>
+      <c r="H687" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="688" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A688" t="s">
+        <v>590</v>
+      </c>
+      <c r="B688" s="4" t="s">
+        <v>602</v>
+      </c>
+      <c r="C688" s="1">
+        <v>44203</v>
+      </c>
+      <c r="D688" t="s">
+        <v>51</v>
+      </c>
+      <c r="E688" t="s">
+        <v>60</v>
+      </c>
+      <c r="F688" t="s">
+        <v>447</v>
+      </c>
+      <c r="H688" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="689" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A689" t="s">
+        <v>590</v>
+      </c>
+      <c r="B689" s="4" t="s">
+        <v>602</v>
+      </c>
+      <c r="C689" s="1">
+        <v>44203</v>
+      </c>
+      <c r="D689" t="s">
+        <v>51</v>
+      </c>
+      <c r="E689" t="s">
+        <v>60</v>
+      </c>
+      <c r="F689" t="s">
+        <v>447</v>
+      </c>
+      <c r="G689" t="s">
+        <v>13</v>
+      </c>
+      <c r="H689" t="s">
+        <v>266</v>
+      </c>
+      <c r="I689" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="690" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A690" t="s">
+        <v>590</v>
+      </c>
+      <c r="B690" s="4" t="s">
+        <v>603</v>
+      </c>
+      <c r="C690" s="1">
+        <v>44201</v>
+      </c>
+      <c r="D690" t="s">
+        <v>167</v>
+      </c>
+      <c r="E690" t="s">
+        <v>51</v>
+      </c>
+      <c r="F690" t="s">
+        <v>447</v>
+      </c>
+      <c r="H690" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="691" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A691" t="s">
+        <v>590</v>
+      </c>
+      <c r="B691" s="4" t="s">
+        <v>604</v>
+      </c>
+      <c r="C691" s="1">
+        <v>44201</v>
+      </c>
+      <c r="D691" t="s">
+        <v>167</v>
+      </c>
+      <c r="E691" t="s">
+        <v>605</v>
+      </c>
+      <c r="F691" t="s">
+        <v>593</v>
+      </c>
+      <c r="H691" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="692" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A692" t="s">
+        <v>590</v>
+      </c>
+      <c r="B692" s="4" t="s">
+        <v>606</v>
+      </c>
+      <c r="C692" s="1">
+        <v>44203</v>
+      </c>
+      <c r="D692" t="s">
+        <v>51</v>
+      </c>
+      <c r="E692" t="s">
+        <v>447</v>
+      </c>
+      <c r="F692" t="s">
+        <v>607</v>
+      </c>
+      <c r="G692" t="s">
+        <v>13</v>
+      </c>
+      <c r="H692" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="693" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A693" t="s">
+        <v>590</v>
+      </c>
+      <c r="B693" s="4" t="s">
+        <v>606</v>
+      </c>
+      <c r="C693" s="1">
+        <v>44203</v>
+      </c>
+      <c r="D693" t="s">
+        <v>51</v>
+      </c>
+      <c r="E693" t="s">
+        <v>447</v>
+      </c>
+      <c r="F693" t="s">
+        <v>607</v>
+      </c>
+      <c r="H693" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="694" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A694" t="s">
+        <v>590</v>
+      </c>
+      <c r="B694" s="4" t="s">
+        <v>608</v>
+      </c>
+      <c r="C694" s="1">
+        <v>44204</v>
+      </c>
+      <c r="D694" t="s">
+        <v>195</v>
+      </c>
+      <c r="E694" t="s">
+        <v>131</v>
+      </c>
+      <c r="F694" t="s">
+        <v>444</v>
+      </c>
+      <c r="H694" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="695" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A695" t="s">
+        <v>590</v>
+      </c>
+      <c r="B695" s="4" t="s">
+        <v>609</v>
+      </c>
+      <c r="C695" s="1">
+        <v>44202</v>
+      </c>
+      <c r="D695" t="s">
+        <v>77</v>
+      </c>
+      <c r="E695" t="s">
+        <v>610</v>
+      </c>
+      <c r="F695" t="s">
+        <v>60</v>
+      </c>
+      <c r="G695" t="s">
+        <v>269</v>
+      </c>
+      <c r="H695" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="696" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A696" t="s">
+        <v>590</v>
+      </c>
+      <c r="B696" s="4" t="s">
+        <v>609</v>
+      </c>
+      <c r="C696" s="1">
+        <v>44202</v>
+      </c>
+      <c r="D696" t="s">
+        <v>77</v>
+      </c>
+      <c r="E696" t="s">
+        <v>610</v>
+      </c>
+      <c r="F696" t="s">
+        <v>60</v>
+      </c>
+      <c r="G696" t="s">
+        <v>477</v>
+      </c>
+      <c r="H696" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="697" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A697" t="s">
+        <v>590</v>
+      </c>
+      <c r="B697" s="8" t="s">
+        <v>609</v>
+      </c>
+      <c r="C697" s="9">
+        <v>44202</v>
+      </c>
+      <c r="D697" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E697" s="10" t="s">
+        <v>610</v>
+      </c>
+      <c r="F697" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="G697" s="10"/>
+      <c r="H697" s="10" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="698" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A698" t="s">
+        <v>590</v>
+      </c>
+      <c r="B698" s="4" t="s">
+        <v>611</v>
+      </c>
+      <c r="C698" s="1">
+        <v>44202</v>
+      </c>
+      <c r="D698" t="s">
+        <v>526</v>
+      </c>
+      <c r="E698" t="s">
+        <v>51</v>
+      </c>
+      <c r="F698" t="s">
+        <v>447</v>
+      </c>
+      <c r="H698" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="699" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A699" t="s">
+        <v>590</v>
+      </c>
+      <c r="B699" s="4" t="s">
+        <v>611</v>
+      </c>
+      <c r="C699" s="1">
+        <v>44202</v>
+      </c>
+      <c r="D699" t="s">
+        <v>526</v>
+      </c>
+      <c r="E699" t="s">
+        <v>51</v>
+      </c>
+      <c r="F699" t="s">
+        <v>447</v>
+      </c>
+      <c r="G699" t="s">
+        <v>13</v>
+      </c>
+      <c r="H699" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="700" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A700" t="s">
+        <v>65</v>
+      </c>
+      <c r="B700" s="4" t="s">
+        <v>437</v>
+      </c>
+      <c r="C700" s="1">
+        <v>44204</v>
+      </c>
+      <c r="D700" t="s">
+        <v>351</v>
+      </c>
+      <c r="E700" t="s">
+        <v>60</v>
+      </c>
+      <c r="F700" t="s">
+        <v>163</v>
+      </c>
+      <c r="H700" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="701" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A701" t="s">
+        <v>65</v>
+      </c>
+      <c r="B701" s="4" t="s">
+        <v>612</v>
+      </c>
+      <c r="C701" s="1">
+        <v>44204</v>
+      </c>
+      <c r="D701" t="s">
+        <v>72</v>
+      </c>
+      <c r="E701" t="s">
+        <v>24</v>
+      </c>
+      <c r="H701" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="702" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A702" t="s">
+        <v>65</v>
+      </c>
+      <c r="B702" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="C702" s="1">
+        <v>44204</v>
+      </c>
+      <c r="D702" t="s">
+        <v>24</v>
+      </c>
+      <c r="E702" t="s">
+        <v>63</v>
+      </c>
+      <c r="F702" t="s">
+        <v>22</v>
+      </c>
+      <c r="H702" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="703" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A703" t="s">
+        <v>65</v>
+      </c>
+      <c r="B703" s="4" t="s">
+        <v>613</v>
+      </c>
+      <c r="C703" s="1">
+        <v>44204</v>
+      </c>
+      <c r="D703" t="s">
+        <v>24</v>
+      </c>
+      <c r="E703" t="s">
+        <v>131</v>
+      </c>
+      <c r="H703" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="704" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A704" t="s">
+        <v>65</v>
+      </c>
+      <c r="B704" s="4" t="s">
+        <v>614</v>
+      </c>
+      <c r="C704" s="1">
+        <v>44204</v>
+      </c>
+      <c r="D704" t="s">
+        <v>78</v>
+      </c>
+      <c r="E704" t="s">
+        <v>24</v>
+      </c>
+      <c r="H704" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="705" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A705" t="s">
+        <v>65</v>
+      </c>
+      <c r="B705" s="4" t="s">
+        <v>615</v>
+      </c>
+      <c r="C705" s="1">
+        <v>44204</v>
+      </c>
+      <c r="D705" t="s">
+        <v>257</v>
+      </c>
+      <c r="H705" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="706" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A706" t="s">
+        <v>65</v>
+      </c>
+      <c r="B706" s="4" t="s">
+        <v>616</v>
+      </c>
+      <c r="C706" s="1">
+        <v>44204</v>
+      </c>
+      <c r="D706" t="s">
+        <v>617</v>
+      </c>
+      <c r="E706" t="s">
+        <v>24</v>
+      </c>
+      <c r="H706" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="707" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A707" t="s">
+        <v>9</v>
+      </c>
+      <c r="B707" s="4" t="s">
+        <v>618</v>
+      </c>
+      <c r="C707" s="1">
+        <v>44176</v>
+      </c>
+      <c r="D707" t="s">
+        <v>151</v>
+      </c>
+      <c r="E707" t="s">
+        <v>22</v>
+      </c>
+      <c r="F707" t="s">
+        <v>24</v>
+      </c>
+      <c r="H707" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="708" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A708" t="s">
+        <v>9</v>
+      </c>
+      <c r="B708" s="4" t="s">
+        <v>619</v>
+      </c>
+      <c r="C708" s="1">
+        <v>44176</v>
+      </c>
+      <c r="D708" t="s">
+        <v>36</v>
+      </c>
+      <c r="E708" t="s">
+        <v>620</v>
+      </c>
+      <c r="H708" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="709" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A709" t="s">
+        <v>9</v>
+      </c>
+      <c r="B709" s="4" t="s">
+        <v>621</v>
+      </c>
+      <c r="C709" s="1">
+        <v>44176</v>
+      </c>
+      <c r="D709" t="s">
+        <v>83</v>
+      </c>
+      <c r="E709" t="s">
+        <v>526</v>
+      </c>
+      <c r="H709" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="710" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A710" t="s">
+        <v>9</v>
+      </c>
+      <c r="B710" s="4" t="s">
+        <v>619</v>
+      </c>
+      <c r="C710" s="1">
+        <v>44176</v>
+      </c>
+      <c r="D710" t="s">
+        <v>168</v>
+      </c>
+      <c r="E710" t="s">
+        <v>622</v>
+      </c>
+      <c r="F710" t="s">
+        <v>60</v>
+      </c>
+      <c r="H710" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="711" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A711" t="s">
+        <v>9</v>
+      </c>
+      <c r="B711" s="4" t="s">
+        <v>623</v>
+      </c>
+      <c r="C711" s="1">
+        <v>44176</v>
+      </c>
+      <c r="D711" t="s">
+        <v>63</v>
+      </c>
+      <c r="E711" t="s">
+        <v>11</v>
+      </c>
+      <c r="F711" t="s">
+        <v>435</v>
+      </c>
+      <c r="H711" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="712" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A712" t="s">
+        <v>9</v>
+      </c>
+      <c r="B712" s="4" t="s">
+        <v>619</v>
+      </c>
+      <c r="C712" s="1">
+        <v>44176</v>
+      </c>
+      <c r="D712" t="s">
+        <v>163</v>
+      </c>
+      <c r="E712" t="s">
+        <v>24</v>
+      </c>
+      <c r="F712" t="s">
+        <v>593</v>
+      </c>
+      <c r="H712" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="713" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A713" t="s">
+        <v>9</v>
+      </c>
+      <c r="B713" s="4" t="s">
+        <v>624</v>
+      </c>
+      <c r="C713" s="1">
+        <v>44176</v>
+      </c>
+      <c r="D713" t="s">
+        <v>625</v>
+      </c>
+      <c r="E713" t="s">
+        <v>62</v>
+      </c>
+      <c r="F713" t="s">
+        <v>265</v>
+      </c>
+      <c r="H713" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="714" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A714" t="s">
+        <v>9</v>
+      </c>
+      <c r="B714" s="4" t="s">
+        <v>626</v>
+      </c>
+      <c r="C714" s="1">
+        <v>44175</v>
+      </c>
+      <c r="D714" t="s">
+        <v>627</v>
+      </c>
+      <c r="E714" t="s">
+        <v>10</v>
+      </c>
+      <c r="F714" t="s">
+        <v>42</v>
+      </c>
+      <c r="H714" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="715" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A715" t="s">
+        <v>9</v>
+      </c>
+      <c r="B715" s="4" t="s">
+        <v>628</v>
+      </c>
+      <c r="C715" s="1">
+        <v>44175</v>
+      </c>
+      <c r="D715" t="s">
+        <v>24</v>
+      </c>
+      <c r="E715" t="s">
+        <v>189</v>
+      </c>
+      <c r="H715" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="716" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A716" t="s">
+        <v>9</v>
+      </c>
+      <c r="B716" s="4" t="s">
+        <v>629</v>
+      </c>
+      <c r="C716" s="1">
+        <v>44175</v>
+      </c>
+      <c r="D716" t="s">
+        <v>19</v>
+      </c>
+      <c r="E716" t="s">
+        <v>630</v>
+      </c>
+      <c r="H716" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="717" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A717" t="s">
+        <v>9</v>
+      </c>
+      <c r="B717" s="4" t="s">
+        <v>631</v>
+      </c>
+      <c r="C717" s="1">
+        <v>44175</v>
+      </c>
+      <c r="D717" t="s">
+        <v>60</v>
+      </c>
+      <c r="E717" t="s">
+        <v>195</v>
+      </c>
+      <c r="G717" t="s">
+        <v>199</v>
+      </c>
+      <c r="H717" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="718" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A718" t="s">
+        <v>9</v>
+      </c>
+      <c r="B718" s="4" t="s">
+        <v>632</v>
+      </c>
+      <c r="C718" s="1">
+        <v>44175</v>
+      </c>
+      <c r="D718" t="s">
+        <v>233</v>
+      </c>
+      <c r="E718" t="s">
+        <v>194</v>
+      </c>
+      <c r="H718" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="719" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A719" t="s">
+        <v>65</v>
+      </c>
+      <c r="B719" s="4" t="s">
+        <v>633</v>
+      </c>
+      <c r="C719" s="1">
+        <v>44183</v>
+      </c>
+      <c r="D719" t="s">
+        <v>634</v>
+      </c>
+      <c r="H719" t="s">
+        <v>69</v>
+      </c>
+      <c r="J719">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="720" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A720" t="s">
+        <v>65</v>
+      </c>
+      <c r="B720" s="4" t="s">
+        <v>438</v>
+      </c>
+      <c r="C720" s="1">
+        <v>44183</v>
+      </c>
+      <c r="D720" t="s">
+        <v>24</v>
+      </c>
+      <c r="E720" t="s">
+        <v>12</v>
+      </c>
+      <c r="F720" t="s">
+        <v>22</v>
+      </c>
+      <c r="H720" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="721" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A721" t="s">
+        <v>590</v>
+      </c>
+      <c r="B721" s="4" t="s">
+        <v>636</v>
+      </c>
+      <c r="C721" s="1">
+        <v>43841</v>
+      </c>
+      <c r="D721" t="s">
+        <v>60</v>
+      </c>
+      <c r="E721" t="s">
+        <v>51</v>
+      </c>
+      <c r="F721" t="s">
+        <v>388</v>
+      </c>
+      <c r="H721" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="722" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A722" t="s">
+        <v>590</v>
+      </c>
+      <c r="B722" s="4" t="s">
+        <v>611</v>
+      </c>
+      <c r="C722" s="1">
+        <v>44209</v>
+      </c>
+      <c r="D722" t="s">
+        <v>526</v>
+      </c>
+      <c r="E722" t="s">
+        <v>193</v>
+      </c>
+      <c r="F722" t="s">
+        <v>73</v>
+      </c>
+      <c r="H722" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="723" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A723" t="s">
+        <v>590</v>
+      </c>
+      <c r="B723" s="4" t="s">
+        <v>603</v>
+      </c>
+      <c r="C723" s="1">
+        <v>44209</v>
+      </c>
+      <c r="D723" t="s">
+        <v>51</v>
+      </c>
+      <c r="E723" t="s">
+        <v>168</v>
+      </c>
+      <c r="F723" t="s">
+        <v>167</v>
+      </c>
+      <c r="H723" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="724" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A724" t="s">
+        <v>590</v>
+      </c>
+      <c r="B724" s="4" t="s">
+        <v>604</v>
+      </c>
+      <c r="C724" s="1">
+        <v>44209</v>
+      </c>
+      <c r="D724" t="s">
+        <v>24</v>
+      </c>
+      <c r="E724" t="s">
+        <v>167</v>
+      </c>
+      <c r="F724" t="s">
+        <v>637</v>
+      </c>
+      <c r="H724" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="725" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A725" t="s">
+        <v>590</v>
+      </c>
+      <c r="B725" s="4" t="s">
+        <v>606</v>
+      </c>
+      <c r="C725" s="1">
+        <v>44209</v>
+      </c>
+      <c r="D725" t="s">
+        <v>49</v>
+      </c>
+      <c r="E725" t="s">
+        <v>24</v>
+      </c>
+      <c r="F725" t="s">
+        <v>51</v>
+      </c>
+      <c r="H725" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="726" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A726" t="s">
+        <v>590</v>
+      </c>
+      <c r="B726" s="4" t="s">
+        <v>638</v>
+      </c>
+      <c r="C726" s="1">
+        <v>44211</v>
+      </c>
+      <c r="D726" t="s">
+        <v>60</v>
+      </c>
+      <c r="E726" t="s">
+        <v>51</v>
+      </c>
+      <c r="F726" t="s">
+        <v>639</v>
+      </c>
+      <c r="H726" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="727" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A727" t="s">
+        <v>9</v>
+      </c>
+      <c r="B727" s="4" t="s">
+        <v>640</v>
+      </c>
+      <c r="C727" s="1">
+        <v>44215</v>
+      </c>
+    </row>
+    <row r="728" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A728" t="s">
+        <v>9</v>
+      </c>
+      <c r="B728" s="4" t="s">
+        <v>641</v>
+      </c>
+      <c r="C728" s="1">
+        <v>44215</v>
+      </c>
+      <c r="D728" t="s">
+        <v>642</v>
+      </c>
+      <c r="E728" t="s">
+        <v>163</v>
+      </c>
+      <c r="F728" t="s">
+        <v>233</v>
+      </c>
+      <c r="G728" t="s">
+        <v>75</v>
+      </c>
+      <c r="H728" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="729" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A729" t="s">
+        <v>9</v>
+      </c>
+      <c r="B729" s="4" t="s">
+        <v>641</v>
+      </c>
+      <c r="C729" s="1">
+        <v>44215</v>
+      </c>
+      <c r="D729" t="s">
+        <v>642</v>
+      </c>
+      <c r="E729" t="s">
+        <v>163</v>
+      </c>
+      <c r="F729" t="s">
+        <v>233</v>
+      </c>
+      <c r="G729" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="730" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A730" t="s">
+        <v>9</v>
+      </c>
+      <c r="B730" s="4" t="s">
+        <v>643</v>
+      </c>
+      <c r="C730" s="1">
+        <v>44215</v>
+      </c>
+      <c r="D730" t="s">
+        <v>149</v>
+      </c>
+      <c r="E730" t="s">
+        <v>79</v>
+      </c>
+      <c r="G730" t="s">
+        <v>75</v>
+      </c>
+      <c r="H730" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="731" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A731" t="s">
+        <v>9</v>
+      </c>
+      <c r="B731" s="4" t="s">
+        <v>643</v>
+      </c>
+      <c r="C731" s="1">
+        <v>44215</v>
+      </c>
+      <c r="D731" t="s">
+        <v>149</v>
+      </c>
+      <c r="E731" t="s">
+        <v>79</v>
+      </c>
+      <c r="G731" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="732" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A732" t="s">
+        <v>9</v>
+      </c>
+      <c r="B732" s="4" t="s">
+        <v>644</v>
+      </c>
+      <c r="C732" s="1">
+        <v>44215</v>
+      </c>
+      <c r="D732" t="s">
+        <v>36</v>
+      </c>
+      <c r="G732" t="s">
+        <v>75</v>
+      </c>
+      <c r="H732" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="733" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A733" t="s">
+        <v>9</v>
+      </c>
+      <c r="B733" s="4" t="s">
+        <v>644</v>
+      </c>
+      <c r="C733" s="1">
+        <v>44215</v>
+      </c>
+      <c r="D733" t="s">
+        <v>36</v>
+      </c>
+      <c r="G733" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="734" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A734" t="s">
+        <v>9</v>
+      </c>
+      <c r="B734" s="4" t="s">
+        <v>645</v>
+      </c>
+      <c r="C734" s="1">
+        <v>44215</v>
+      </c>
+      <c r="G734" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="735" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A735" t="s">
+        <v>9</v>
+      </c>
+      <c r="B735" s="4" t="s">
+        <v>646</v>
+      </c>
+      <c r="C735" s="1">
+        <v>44215</v>
+      </c>
+      <c r="G735" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="736" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A736" t="s">
+        <v>9</v>
+      </c>
+      <c r="B736" s="4" t="s">
+        <v>647</v>
+      </c>
+      <c r="C736" s="1">
+        <v>44215</v>
+      </c>
+      <c r="G736" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="737" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A737" t="s">
+        <v>9</v>
+      </c>
+      <c r="B737" s="4" t="s">
+        <v>648</v>
+      </c>
+      <c r="C737" s="1">
+        <v>44215</v>
+      </c>
+      <c r="G737" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="738" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A738" t="s">
+        <v>9</v>
+      </c>
+      <c r="B738" s="4" t="s">
+        <v>649</v>
+      </c>
+      <c r="C738" s="1">
+        <v>44215</v>
+      </c>
+      <c r="G738" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="739" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A739" t="s">
+        <v>9</v>
+      </c>
+      <c r="B739" s="4" t="s">
+        <v>650</v>
+      </c>
+      <c r="C739" s="1">
+        <v>44215</v>
+      </c>
+      <c r="G739" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="740" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A740" t="s">
+        <v>9</v>
+      </c>
+      <c r="B740" s="4" t="s">
+        <v>651</v>
+      </c>
+      <c r="C740" s="1">
+        <v>44215</v>
+      </c>
+      <c r="G740" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="741" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A741" t="s">
+        <v>9</v>
+      </c>
+      <c r="B741" s="4" t="s">
+        <v>652</v>
+      </c>
+      <c r="C741" s="1">
+        <v>44215</v>
+      </c>
+      <c r="G741" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="742" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A742" t="s">
+        <v>9</v>
+      </c>
+      <c r="B742" s="4" t="s">
+        <v>653</v>
+      </c>
+      <c r="C742" s="1">
+        <v>44215</v>
+      </c>
+      <c r="G742" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="743" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A743" t="s">
+        <v>9</v>
+      </c>
+      <c r="B743" s="4" t="s">
+        <v>654</v>
+      </c>
+      <c r="C743" s="1">
+        <v>44215</v>
+      </c>
+      <c r="G743" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="744" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A744" t="s">
+        <v>9</v>
+      </c>
+      <c r="B744" s="4" t="s">
+        <v>655</v>
+      </c>
+      <c r="C744" s="1">
+        <v>44215</v>
+      </c>
+      <c r="G744" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="745" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A745" t="s">
+        <v>9</v>
+      </c>
+      <c r="B745" s="4" t="s">
+        <v>656</v>
+      </c>
+      <c r="C745" s="1">
+        <v>44215</v>
+      </c>
+      <c r="G745" t="s">
+        <v>125</v>
+      </c>
+      <c r="H745" t="s">
+        <v>126</v>
+      </c>
+      <c r="I745" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="746" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A746" t="s">
+        <v>9</v>
+      </c>
+      <c r="B746" s="4" t="s">
+        <v>657</v>
+      </c>
+      <c r="C746" s="1">
+        <v>44215</v>
+      </c>
+      <c r="G746" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="747" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A747" t="s">
+        <v>9</v>
+      </c>
+      <c r="B747" s="4" t="s">
+        <v>658</v>
+      </c>
+      <c r="C747" s="1">
+        <v>44216</v>
+      </c>
+      <c r="G747" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="748" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A748" t="s">
+        <v>9</v>
+      </c>
+      <c r="B748" s="4" t="s">
+        <v>659</v>
+      </c>
+      <c r="C748" s="1">
+        <v>44216</v>
+      </c>
+      <c r="G748" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="749" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A749" t="s">
+        <v>9</v>
+      </c>
+      <c r="B749" s="4" t="s">
+        <v>660</v>
+      </c>
+      <c r="C749" s="1">
+        <v>44216</v>
+      </c>
+      <c r="G749" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="750" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A750" t="s">
+        <v>9</v>
+      </c>
+      <c r="B750" s="4" t="s">
+        <v>661</v>
+      </c>
+      <c r="C750" s="1">
+        <v>44216</v>
+      </c>
+      <c r="G750" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="751" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A751" t="s">
+        <v>9</v>
+      </c>
+      <c r="B751" s="4" t="s">
+        <v>662</v>
+      </c>
+      <c r="C751" s="1">
+        <v>44216</v>
+      </c>
+      <c r="G751" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="752" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A752" t="s">
+        <v>9</v>
+      </c>
+      <c r="B752" s="4" t="s">
+        <v>663</v>
+      </c>
+      <c r="C752" s="1">
+        <v>44216</v>
+      </c>
+      <c r="G752" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="753" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A753" t="s">
+        <v>9</v>
+      </c>
+      <c r="B753" s="4" t="s">
+        <v>664</v>
+      </c>
+      <c r="C753" s="1">
+        <v>44216</v>
+      </c>
+      <c r="G753" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="754" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A754" t="s">
+        <v>9</v>
+      </c>
+      <c r="B754" s="4" t="s">
+        <v>665</v>
+      </c>
+      <c r="C754" s="1">
+        <v>44216</v>
+      </c>
+      <c r="D754" t="s">
+        <v>42</v>
+      </c>
+      <c r="E754" t="s">
+        <v>666</v>
+      </c>
+      <c r="F754" t="s">
+        <v>43</v>
+      </c>
+      <c r="G754" t="s">
+        <v>75</v>
+      </c>
+      <c r="H754" t="s">
+        <v>91</v>
+      </c>
+      <c r="I754" t="s">
+        <v>667</v>
+      </c>
+      <c r="J754">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="755" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A755" t="s">
+        <v>9</v>
+      </c>
+      <c r="B755" s="4" t="s">
+        <v>665</v>
+      </c>
+      <c r="C755" s="1">
+        <v>44216</v>
+      </c>
+      <c r="D755" t="s">
+        <v>42</v>
+      </c>
+      <c r="E755" t="s">
+        <v>666</v>
+      </c>
+      <c r="F755" t="s">
+        <v>43</v>
+      </c>
+      <c r="G755" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="756" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A756" t="s">
+        <v>9</v>
+      </c>
+      <c r="B756" s="4" t="s">
+        <v>668</v>
+      </c>
+      <c r="C756" s="1">
+        <v>44217</v>
+      </c>
+      <c r="G756" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="757" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A757" t="s">
+        <v>9</v>
+      </c>
+      <c r="B757" s="4" t="s">
+        <v>669</v>
+      </c>
+      <c r="C757" s="1">
+        <v>44217</v>
+      </c>
+      <c r="G757" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="758" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A758" t="s">
+        <v>9</v>
+      </c>
+      <c r="B758" s="4" t="s">
+        <v>670</v>
+      </c>
+      <c r="C758" s="1">
+        <v>44217</v>
+      </c>
+      <c r="G758" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="759" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A759" t="s">
+        <v>9</v>
+      </c>
+      <c r="B759" s="4" t="s">
+        <v>671</v>
+      </c>
+      <c r="C759" s="1">
+        <v>44217</v>
+      </c>
+      <c r="G759" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="760" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A760" t="s">
+        <v>9</v>
+      </c>
+      <c r="B760" s="4" t="s">
+        <v>672</v>
+      </c>
+      <c r="C760" s="1">
+        <v>44217</v>
+      </c>
+      <c r="G760" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="761" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A761" t="s">
+        <v>9</v>
+      </c>
+      <c r="B761" s="4" t="s">
+        <v>673</v>
+      </c>
+      <c r="C761" s="1">
+        <v>44217</v>
+      </c>
+      <c r="G761" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="762" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A762" t="s">
+        <v>9</v>
+      </c>
+      <c r="B762" s="4" t="s">
+        <v>674</v>
+      </c>
+      <c r="C762" s="1">
+        <v>44217</v>
+      </c>
+      <c r="G762" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="763" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A763" t="s">
+        <v>9</v>
+      </c>
+      <c r="B763" s="4" t="s">
+        <v>675</v>
+      </c>
+      <c r="C763" s="1">
+        <v>44217</v>
+      </c>
+      <c r="G763" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="764" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A764" t="s">
+        <v>9</v>
+      </c>
+      <c r="B764" s="4" t="s">
+        <v>676</v>
+      </c>
+      <c r="C764" s="1">
+        <v>44217</v>
+      </c>
+      <c r="G764" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="765" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A765" t="s">
+        <v>9</v>
+      </c>
+      <c r="B765" s="4" t="s">
+        <v>677</v>
+      </c>
+      <c r="C765" s="1">
+        <v>44217</v>
+      </c>
+      <c r="G765" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="766" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A766" t="s">
+        <v>9</v>
+      </c>
+      <c r="B766" s="4" t="s">
+        <v>678</v>
+      </c>
+      <c r="C766" s="1">
+        <v>44217</v>
+      </c>
+      <c r="G766" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="767" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A767" t="s">
+        <v>9</v>
+      </c>
+      <c r="B767" s="4" t="s">
+        <v>679</v>
+      </c>
+      <c r="C767" s="1">
+        <v>44217</v>
+      </c>
+      <c r="G767" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="768" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A768" t="s">
+        <v>9</v>
+      </c>
+      <c r="B768" s="4" t="s">
+        <v>680</v>
+      </c>
+      <c r="C768" s="1">
+        <v>44217</v>
+      </c>
+      <c r="G768" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="769" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A769" t="s">
+        <v>9</v>
+      </c>
+      <c r="B769" s="4" t="s">
+        <v>681</v>
+      </c>
+      <c r="C769" s="1">
+        <v>44217</v>
+      </c>
+      <c r="D769" t="s">
+        <v>682</v>
+      </c>
+      <c r="E769" t="s">
+        <v>116</v>
+      </c>
+      <c r="F769" t="s">
+        <v>79</v>
+      </c>
+      <c r="G769" t="s">
+        <v>75</v>
+      </c>
+      <c r="H769" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="770" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A770" t="s">
+        <v>9</v>
+      </c>
+      <c r="B770" s="4" t="s">
+        <v>681</v>
+      </c>
+      <c r="C770" s="1">
+        <v>44217</v>
+      </c>
+      <c r="D770" t="s">
+        <v>682</v>
+      </c>
+      <c r="E770" t="s">
+        <v>116</v>
+      </c>
+      <c r="F770" t="s">
+        <v>79</v>
+      </c>
+      <c r="G770" t="s">
+        <v>75</v>
+      </c>
+      <c r="H770" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="771" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A771" t="s">
+        <v>9</v>
+      </c>
+      <c r="B771" s="4" t="s">
+        <v>683</v>
+      </c>
+      <c r="C771" s="1">
+        <v>44217</v>
+      </c>
+      <c r="D771" t="s">
+        <v>131</v>
+      </c>
+      <c r="G771" t="s">
+        <v>125</v>
+      </c>
+      <c r="H771" t="s">
+        <v>127</v>
+      </c>
+      <c r="I771" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="772" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A772" t="s">
+        <v>9</v>
+      </c>
+      <c r="B772" s="4" t="s">
+        <v>684</v>
+      </c>
+      <c r="C772" s="1">
+        <v>44217</v>
+      </c>
+      <c r="G772" t="s">
+        <v>125</v>
+      </c>
+      <c r="H772" t="s">
+        <v>126</v>
+      </c>
+      <c r="I772" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="773" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A773" t="s">
+        <v>9</v>
+      </c>
+      <c r="B773" s="4" t="s">
+        <v>685</v>
+      </c>
+      <c r="C773" s="1">
+        <v>44217</v>
+      </c>
+      <c r="G773" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="774" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A774" t="s">
+        <v>9</v>
+      </c>
+      <c r="B774" s="4" t="s">
+        <v>686</v>
+      </c>
+      <c r="C774" s="1">
+        <v>44217</v>
+      </c>
+      <c r="G774" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="775" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A775" t="s">
+        <v>9</v>
+      </c>
+      <c r="B775" s="4" t="s">
+        <v>687</v>
+      </c>
+      <c r="C775" s="1">
+        <v>44217</v>
+      </c>
+      <c r="G775" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="776" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A776" t="s">
+        <v>9</v>
+      </c>
+      <c r="B776" s="4" t="s">
+        <v>688</v>
+      </c>
+      <c r="C776" s="1">
+        <v>44217</v>
+      </c>
+      <c r="G776" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="777" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A777" t="s">
+        <v>9</v>
+      </c>
+      <c r="B777" s="4" t="s">
+        <v>689</v>
+      </c>
+      <c r="C777" s="1">
+        <v>44217</v>
+      </c>
+      <c r="G777" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="778" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A778" t="s">
+        <v>9</v>
+      </c>
+      <c r="B778" s="4" t="s">
+        <v>690</v>
+      </c>
+      <c r="C778" s="1">
+        <v>44217</v>
+      </c>
+      <c r="G778" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="779" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A779" t="s">
+        <v>9</v>
+      </c>
+      <c r="B779" s="4" t="s">
+        <v>691</v>
+      </c>
+      <c r="C779" s="1">
+        <v>44223</v>
+      </c>
+      <c r="G779" t="s">
+        <v>75</v>
+      </c>
+      <c r="H779" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="780" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A780" t="s">
+        <v>9</v>
+      </c>
+      <c r="B780" s="4" t="s">
+        <v>692</v>
+      </c>
+      <c r="C780" s="1">
+        <v>44223</v>
+      </c>
+      <c r="G780" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="781" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A781" t="s">
+        <v>9</v>
+      </c>
+      <c r="B781" s="4" t="s">
+        <v>693</v>
+      </c>
+      <c r="C781" s="1">
+        <v>44223</v>
+      </c>
+      <c r="G781" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="782" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A782" t="s">
+        <v>9</v>
+      </c>
+      <c r="B782" s="4" t="s">
+        <v>694</v>
+      </c>
+      <c r="C782" s="1">
+        <v>44223</v>
+      </c>
+      <c r="G782" t="s">
+        <v>125</v>
+      </c>
+      <c r="H782" t="s">
+        <v>126</v>
+      </c>
+      <c r="I782" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="783" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A783" t="s">
+        <v>9</v>
+      </c>
+      <c r="B783" s="4" t="s">
+        <v>695</v>
+      </c>
+      <c r="C783" s="1">
+        <v>44223</v>
+      </c>
+      <c r="G783" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="784" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A784" t="s">
+        <v>9</v>
+      </c>
+      <c r="B784" s="4" t="s">
+        <v>691</v>
+      </c>
+      <c r="C784" s="1">
+        <v>44223</v>
+      </c>
+      <c r="G784" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="785" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A785" t="s">
+        <v>9</v>
+      </c>
+      <c r="B785" s="4" t="s">
+        <v>696</v>
+      </c>
+      <c r="C785" s="1">
+        <v>44223</v>
+      </c>
+      <c r="G785" t="s">
+        <v>80</v>
+      </c>
+      <c r="H785" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="786" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A786" t="s">
+        <v>9</v>
+      </c>
+      <c r="B786" s="4" t="s">
+        <v>697</v>
+      </c>
+      <c r="C786" s="1">
+        <v>44223</v>
+      </c>
+      <c r="G786" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="787" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A787" t="s">
+        <v>9</v>
+      </c>
+      <c r="B787" s="4" t="s">
+        <v>698</v>
+      </c>
+      <c r="C787" s="1">
+        <v>44222</v>
+      </c>
+      <c r="G787" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="788" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A788" t="s">
+        <v>9</v>
+      </c>
+      <c r="B788" s="4" t="s">
+        <v>699</v>
+      </c>
+      <c r="C788" s="1">
+        <v>44222</v>
+      </c>
+      <c r="G788" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="789" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A789" t="s">
+        <v>9</v>
+      </c>
+      <c r="B789" s="4" t="s">
+        <v>700</v>
+      </c>
+      <c r="C789" s="1">
+        <v>44222</v>
+      </c>
+      <c r="G789" t="s">
+        <v>80</v>
+      </c>
+      <c r="H789" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="790" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A790" t="s">
+        <v>9</v>
+      </c>
+      <c r="B790" s="4" t="s">
+        <v>701</v>
+      </c>
+      <c r="C790" s="1">
+        <v>44222</v>
+      </c>
+      <c r="G790" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="791" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A791" t="s">
+        <v>9</v>
+      </c>
+      <c r="B791" s="4" t="s">
+        <v>684</v>
+      </c>
+      <c r="C791" s="1">
+        <v>44222</v>
+      </c>
+      <c r="G791" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="792" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A792" t="s">
+        <v>9</v>
+      </c>
+      <c r="B792" s="4" t="s">
+        <v>702</v>
+      </c>
+      <c r="C792" s="1">
+        <v>44222</v>
+      </c>
+      <c r="G792" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="793" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A793" t="s">
+        <v>9</v>
+      </c>
+      <c r="B793" s="4" t="s">
+        <v>703</v>
+      </c>
+      <c r="C793" s="1">
+        <v>44222</v>
+      </c>
+      <c r="G793" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="794" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A794" t="s">
+        <v>9</v>
+      </c>
+      <c r="B794" s="4" t="s">
+        <v>696</v>
+      </c>
+      <c r="C794" s="1">
+        <v>44222</v>
+      </c>
+      <c r="D794" t="s">
+        <v>136</v>
+      </c>
+      <c r="E794" t="s">
+        <v>135</v>
+      </c>
+      <c r="F794" t="s">
+        <v>131</v>
+      </c>
+      <c r="G794" t="s">
+        <v>75</v>
+      </c>
+      <c r="H794" t="s">
+        <v>91</v>
+      </c>
+      <c r="I794" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="795" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A795" t="s">
+        <v>9</v>
+      </c>
+      <c r="B795" s="4" t="s">
+        <v>705</v>
+      </c>
+      <c r="C795" s="1">
+        <v>44221</v>
+      </c>
+      <c r="G795" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="796" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A796" t="s">
+        <v>9</v>
+      </c>
+      <c r="B796" s="4" t="s">
+        <v>706</v>
+      </c>
+      <c r="C796" s="1">
+        <v>44221</v>
+      </c>
+      <c r="G796" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="797" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A797" t="s">
+        <v>9</v>
+      </c>
+      <c r="B797" s="4" t="s">
+        <v>707</v>
+      </c>
+      <c r="C797" s="1">
+        <v>44221</v>
+      </c>
+      <c r="G797" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="798" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A798" t="s">
+        <v>9</v>
+      </c>
+      <c r="B798" s="4" t="s">
+        <v>708</v>
+      </c>
+      <c r="C798" s="1">
+        <v>44221</v>
+      </c>
+      <c r="G798" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="799" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A799" t="s">
+        <v>9</v>
+      </c>
+      <c r="B799" s="4" t="s">
+        <v>709</v>
+      </c>
+      <c r="C799" s="1">
+        <v>44221</v>
+      </c>
+      <c r="G799" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="800" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A800" t="s">
+        <v>9</v>
+      </c>
+      <c r="B800" s="4" t="s">
+        <v>710</v>
+      </c>
+      <c r="C800" s="1">
+        <v>44221</v>
+      </c>
+      <c r="G800" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="801" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A801" t="s">
+        <v>9</v>
+      </c>
+      <c r="B801" s="4" t="s">
+        <v>711</v>
+      </c>
+      <c r="C801" s="1">
+        <v>44221</v>
+      </c>
+      <c r="G801" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="802" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A802" t="s">
+        <v>9</v>
+      </c>
+      <c r="B802" s="4" t="s">
+        <v>712</v>
+      </c>
+      <c r="C802" s="1">
+        <v>44221</v>
+      </c>
+      <c r="G802" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="803" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A803" t="s">
+        <v>9</v>
+      </c>
+      <c r="B803" s="4" t="s">
+        <v>713</v>
+      </c>
+      <c r="C803" s="1">
+        <v>44221</v>
+      </c>
+      <c r="G803" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="804" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A804" t="s">
+        <v>9</v>
+      </c>
+      <c r="B804" s="4" t="s">
+        <v>714</v>
+      </c>
+      <c r="C804" s="1">
+        <v>44221</v>
+      </c>
+      <c r="G804" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="805" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A805" t="s">
+        <v>9</v>
+      </c>
+      <c r="B805" s="4" t="s">
+        <v>719</v>
+      </c>
+      <c r="C805" s="1">
+        <v>44221</v>
+      </c>
+      <c r="G805" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="806" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A806" t="s">
+        <v>9</v>
+      </c>
+      <c r="B806" s="4" t="s">
+        <v>715</v>
+      </c>
+      <c r="C806" s="1">
+        <v>44221</v>
+      </c>
+      <c r="G806" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="807" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A807" t="s">
+        <v>9</v>
+      </c>
+      <c r="B807" s="4" t="s">
+        <v>716</v>
+      </c>
+      <c r="C807" s="1">
+        <v>44221</v>
+      </c>
+      <c r="D807" t="s">
+        <v>74</v>
+      </c>
+      <c r="E807" t="s">
+        <v>36</v>
+      </c>
+      <c r="G807" t="s">
+        <v>75</v>
+      </c>
+      <c r="H807" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="808" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A808" t="s">
+        <v>9</v>
+      </c>
+      <c r="B808" s="4" t="s">
+        <v>716</v>
+      </c>
+      <c r="C808" s="1">
+        <v>44221</v>
+      </c>
+      <c r="D808" t="s">
+        <v>74</v>
+      </c>
+      <c r="E808" t="s">
+        <v>36</v>
+      </c>
+      <c r="G808" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="809" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A809" t="s">
+        <v>9</v>
+      </c>
+      <c r="B809" s="4" t="s">
+        <v>717</v>
+      </c>
+      <c r="C809" s="1">
+        <v>44221</v>
+      </c>
+      <c r="G809" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="810" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A810" t="s">
+        <v>9</v>
+      </c>
+      <c r="B810" s="4" t="s">
+        <v>718</v>
+      </c>
+      <c r="C810" s="1">
+        <v>44221</v>
+      </c>
+      <c r="G810" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>